<commit_message>
Don't translate "False" when it is a Python variable
</commit_message>
<xml_diff>
--- a/docassemble/CDCEvictionMoratorium/data/sources/cdc_eviction_moratorium_es.xlsx
+++ b/docassemble/CDCEvictionMoratorium/data/sources/cdc_eviction_moratorium_es.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1824" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2274" uniqueCount="691">
   <si>
     <t>interview</t>
   </si>
@@ -4653,61 +4653,6 @@
     <t>346c3101a9ee699e66c013ffa02da815</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">MassAccess submission from </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>${users}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> intended for </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>${courts[0]}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
     <t>Question_75</t>
   </si>
   <si>
@@ -5387,9 +5332,6 @@
     <t>False</t>
   </si>
   <si>
-    <t>Falso</t>
-  </si>
-  <si>
     <t>3d9bf4309999db58ee3203a0035723bc</t>
   </si>
   <si>
@@ -6594,9 +6536,6 @@
   </si>
   <si>
     <t>¿Cuál es su direccion?</t>
-  </si>
-  <si>
-    <t>dirección</t>
   </si>
   <si>
     <t>Apartamento</t>
@@ -7364,6 +7303,57 @@
   </si>
   <si>
     <t>Para continuar, debe aceptar los [términos de uso](https://massaccess.suffolklitlab.org/privacy/)</t>
+  </si>
+  <si>
+    <t>Dirección</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MassAccess submission from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>${users}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> intended for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>${courts[0]}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -7752,15 +7742,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <pane ySplit="6590" topLeftCell="A252"/>
-      <selection activeCell="H132" sqref="H132"/>
-      <selection pane="bottomLeft" activeCell="H253" sqref="H253"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="H180" sqref="H180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7265625" customWidth="1"/>
+    <col min="1" max="1" width="34.08984375" customWidth="1"/>
     <col min="2" max="2" width="15.7265625" customWidth="1"/>
     <col min="3" max="3" width="12.7265625" customWidth="1"/>
     <col min="7" max="8" width="75.7265625" customWidth="1"/>
@@ -8647,7 +8635,7 @@
         <v>88</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -8673,7 +8661,7 @@
         <v>90</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -8699,7 +8687,7 @@
         <v>92</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
@@ -8725,7 +8713,7 @@
         <v>94</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -8933,7 +8921,7 @@
         <v>112</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.35">
@@ -9063,7 +9051,7 @@
         <v>124</v>
       </c>
       <c r="H50" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
@@ -9089,7 +9077,7 @@
         <v>126</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
@@ -9115,7 +9103,7 @@
         <v>128</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
@@ -9141,7 +9129,7 @@
         <v>130</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -9217,7 +9205,7 @@
         <v>138</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -9269,7 +9257,7 @@
         <v>142</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>654</v>
+        <v>689</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.35">
@@ -9295,7 +9283,7 @@
         <v>144</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.35">
@@ -9321,7 +9309,7 @@
         <v>146</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
@@ -9347,7 +9335,7 @@
         <v>148</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
@@ -9399,7 +9387,7 @@
         <v>152</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -10647,7 +10635,7 @@
         <v>264</v>
       </c>
       <c r="H111" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.35">
@@ -10673,7 +10661,7 @@
         <v>266</v>
       </c>
       <c r="H112" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="113" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.35">
@@ -11089,7 +11077,7 @@
         <v>313</v>
       </c>
       <c r="H128" s="3" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -11115,7 +11103,7 @@
         <v>315</v>
       </c>
       <c r="H129" s="4" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.35">
@@ -11141,7 +11129,7 @@
         <v>317</v>
       </c>
       <c r="H130" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.35">
@@ -11167,7 +11155,7 @@
         <v>319</v>
       </c>
       <c r="H131" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -11193,7 +11181,7 @@
         <v>322</v>
       </c>
       <c r="H132" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="133" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -11788,7 +11776,7 @@
         <v>12</v>
       </c>
       <c r="G155" s="3" t="s">
-        <v>377</v>
+        <v>690</v>
       </c>
       <c r="H155" s="4" t="s">
         <v>14</v>
@@ -11799,22 +11787,22 @@
         <v>8</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C156" s="2">
         <v>0</v>
       </c>
       <c r="D156" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="E156" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F156" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G156" s="3" t="s">
         <v>379</v>
-      </c>
-      <c r="E156" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F156" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G156" s="3" t="s">
-        <v>380</v>
       </c>
       <c r="H156" s="4" t="s">
         <v>14</v>
@@ -11825,22 +11813,22 @@
         <v>8</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C157" s="2">
         <v>1</v>
       </c>
       <c r="D157" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E157" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F157" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G157" s="3" t="s">
         <v>381</v>
-      </c>
-      <c r="E157" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F157" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G157" s="3" t="s">
-        <v>382</v>
       </c>
       <c r="H157" s="4" t="s">
         <v>14</v>
@@ -11851,22 +11839,22 @@
         <v>8</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C158" s="2">
         <v>2</v>
       </c>
       <c r="D158" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="E158" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F158" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G158" s="5" t="s">
         <v>383</v>
-      </c>
-      <c r="E158" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F158" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G158" s="5" t="s">
-        <v>384</v>
       </c>
       <c r="H158" s="4" t="s">
         <v>14</v>
@@ -11877,22 +11865,22 @@
         <v>8</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C159" s="2">
         <v>0</v>
       </c>
       <c r="D159" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="E159" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F159" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G159" s="3" t="s">
         <v>386</v>
-      </c>
-      <c r="E159" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F159" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G159" s="3" t="s">
-        <v>387</v>
       </c>
       <c r="H159" s="4" t="s">
         <v>14</v>
@@ -11903,22 +11891,22 @@
         <v>8</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C160" s="2">
         <v>1</v>
       </c>
       <c r="D160" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E160" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F160" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G160" s="3" t="s">
         <v>388</v>
-      </c>
-      <c r="E160" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F160" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G160" s="3" t="s">
-        <v>389</v>
       </c>
       <c r="H160" s="4" t="s">
         <v>14</v>
@@ -11929,22 +11917,22 @@
         <v>8</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C161" s="2">
         <v>2</v>
       </c>
       <c r="D161" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E161" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F161" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G161" s="3" t="s">
         <v>390</v>
-      </c>
-      <c r="E161" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F161" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G161" s="3" t="s">
-        <v>391</v>
       </c>
       <c r="H161" s="4" t="s">
         <v>14</v>
@@ -11955,22 +11943,22 @@
         <v>8</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C162" s="2">
         <v>3</v>
       </c>
       <c r="D162" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="E162" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F162" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G162" s="3" t="s">
         <v>392</v>
-      </c>
-      <c r="E162" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F162" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G162" s="3" t="s">
-        <v>393</v>
       </c>
       <c r="H162" s="4" t="s">
         <v>14</v>
@@ -11981,25 +11969,25 @@
         <v>8</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C163" s="2">
         <v>0</v>
       </c>
       <c r="D163" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="E163" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F163" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G163" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="E163" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F163" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G163" s="3" t="s">
+      <c r="H163" s="4" t="s">
         <v>396</v>
-      </c>
-      <c r="H163" s="4" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="164" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.35">
@@ -12007,48 +11995,48 @@
         <v>8</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C164" s="2">
         <v>1</v>
       </c>
       <c r="D164" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="E164" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F164" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G164" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="E164" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F164" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G164" s="3" t="s">
+      <c r="H164" s="4" t="s">
         <v>399</v>
-      </c>
-      <c r="H164" s="4" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A165" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B165" s="2" t="s">
         <v>401</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>402</v>
       </c>
       <c r="C165" s="2">
         <v>0</v>
       </c>
       <c r="D165" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="E165" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F165" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G165" s="5" t="s">
         <v>403</v>
-      </c>
-      <c r="E165" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F165" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G165" s="5" t="s">
-        <v>404</v>
       </c>
       <c r="H165" s="4" t="s">
         <v>14</v>
@@ -12056,25 +12044,25 @@
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A166" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B166" s="2" t="s">
         <v>401</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>402</v>
       </c>
       <c r="C166" s="2">
         <v>1</v>
       </c>
       <c r="D166" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="E166" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F166" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G166" s="5" t="s">
         <v>405</v>
-      </c>
-      <c r="E166" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F166" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G166" s="5" t="s">
-        <v>406</v>
       </c>
       <c r="H166" s="4" t="s">
         <v>14</v>
@@ -12082,42 +12070,42 @@
     </row>
     <row r="167" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C167" s="2">
         <v>0</v>
       </c>
       <c r="D167" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F167" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G167" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="E167" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F167" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G167" s="3" t="s">
+      <c r="H167" s="4" t="s">
         <v>409</v>
-      </c>
-      <c r="H167" s="4" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="168" spans="1:8" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C168" s="2">
         <v>1</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E168" s="2" t="s">
         <v>11</v>
@@ -12126,50 +12114,50 @@
         <v>12</v>
       </c>
       <c r="G168" s="3" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="H168" s="4" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
     </row>
     <row r="169" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C169" s="2">
         <v>0</v>
       </c>
       <c r="D169" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="E169" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F169" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G169" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="E169" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F169" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G169" s="3" t="s">
+      <c r="H169" s="4" t="s">
         <v>414</v>
-      </c>
-      <c r="H169" s="4" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="170" spans="1:8" ht="135" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C170" s="2">
         <v>1</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E170" s="2" t="s">
         <v>11</v>
@@ -12178,310 +12166,308 @@
         <v>12</v>
       </c>
       <c r="G170" s="3" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="H170" s="4" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
     </row>
     <row r="171" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C171" s="2">
         <v>2</v>
       </c>
       <c r="D171" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="E171" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F171" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G171" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="E171" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F171" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G171" s="3" t="s">
-        <v>418</v>
-      </c>
       <c r="H171" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
     </row>
     <row r="172" spans="1:8" ht="150" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C172" s="2">
         <v>3</v>
       </c>
       <c r="D172" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="E172" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F172" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G172" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="E172" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F172" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G172" s="3" t="s">
-        <v>420</v>
-      </c>
       <c r="H172" s="4" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
     </row>
     <row r="173" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C173" s="2">
         <v>0</v>
       </c>
       <c r="D173" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="E173" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F173" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G173" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="E173" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F173" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G173" s="3" t="s">
+      <c r="H173" s="4" t="s">
         <v>423</v>
-      </c>
-      <c r="H173" s="4" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="174" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C174" s="2">
         <v>1</v>
       </c>
       <c r="D174" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="E174" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F174" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G174" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="E174" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F174" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G174" s="3" t="s">
-        <v>426</v>
-      </c>
       <c r="H174" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A175" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C175" s="2">
         <v>2</v>
       </c>
       <c r="D175" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="E175" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F175" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G175" s="3" t="s">
         <v>427</v>
       </c>
-      <c r="E175" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F175" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G175" s="3" t="s">
-        <v>428</v>
-      </c>
       <c r="H175" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A176" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C176" s="2">
         <v>3</v>
       </c>
       <c r="D176" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E176" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F176" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G176" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="E176" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F176" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G176" s="3" t="s">
-        <v>430</v>
-      </c>
       <c r="H176" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
     </row>
     <row r="177" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C177" s="2">
         <v>0</v>
       </c>
       <c r="D177" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="E177" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F177" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G177" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="E177" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F177" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G177" s="3" t="s">
-        <v>433</v>
-      </c>
       <c r="H177" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A178" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C178" s="2">
         <v>1</v>
       </c>
       <c r="D178" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="E178" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F178" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G178" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="E178" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F178" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G178" s="3" t="s">
+      <c r="H178" s="4" t="s">
         <v>435</v>
-      </c>
-      <c r="H178" s="4" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A179" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C179" s="2">
         <v>2</v>
       </c>
       <c r="D179" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E179" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F179" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G179" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="E179" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F179" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G179" s="3" t="s">
+      <c r="H179" s="4" t="s">
         <v>438</v>
-      </c>
-      <c r="H179" s="4" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A180" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C180" s="2">
         <v>3</v>
       </c>
       <c r="D180" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="E180" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F180" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G180" s="3" t="s">
         <v>440</v>
       </c>
-      <c r="E180" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F180" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G180" s="3" t="s">
-        <v>441</v>
-      </c>
-      <c r="H180" s="4" t="s">
-        <v>442</v>
-      </c>
+      <c r="H180" s="4"/>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A181" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C181" s="2">
         <v>4</v>
       </c>
       <c r="D181" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="E181" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F181" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G181" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="H181" s="4" t="s">
         <v>443</v>
-      </c>
-      <c r="E181" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F181" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G181" s="3" t="s">
-        <v>444</v>
-      </c>
-      <c r="H181" s="4" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="182" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C182" s="2">
         <v>0</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E182" s="2" t="s">
         <v>11</v>
@@ -12490,24 +12476,24 @@
         <v>12</v>
       </c>
       <c r="G182" s="3" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="H182" s="4" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
     </row>
     <row r="183" spans="1:8" ht="210" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C183" s="2">
         <v>1</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E183" s="2" t="s">
         <v>11</v>
@@ -12516,154 +12502,154 @@
         <v>12</v>
       </c>
       <c r="G183" s="3" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="H183" s="4" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A184" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C184" s="2">
         <v>2</v>
       </c>
       <c r="D184" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="E184" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F184" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G184" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="H184" s="4" t="s">
         <v>450</v>
-      </c>
-      <c r="E184" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F184" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G184" s="3" t="s">
-        <v>451</v>
-      </c>
-      <c r="H184" s="4" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A185" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C185" s="2">
         <v>3</v>
       </c>
       <c r="D185" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E185" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F185" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G185" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="H185" s="4" t="s">
         <v>453</v>
-      </c>
-      <c r="E185" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F185" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G185" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="H185" s="4" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="186" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C186" s="2">
         <v>0</v>
       </c>
       <c r="D186" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="E186" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F186" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G186" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="H186" s="4" t="s">
         <v>457</v>
-      </c>
-      <c r="E186" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F186" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G186" s="3" t="s">
-        <v>458</v>
-      </c>
-      <c r="H186" s="4" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="187" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C187" s="2">
         <v>1</v>
       </c>
       <c r="D187" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="E187" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F187" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G187" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="H187" s="4" t="s">
         <v>460</v>
-      </c>
-      <c r="E187" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F187" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G187" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="H187" s="4" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="188" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C188" s="2">
         <v>2</v>
       </c>
       <c r="D188" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="E188" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F188" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G188" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="H188" s="4" t="s">
         <v>463</v>
-      </c>
-      <c r="E188" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F188" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G188" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="H188" s="4" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="189" spans="1:8" ht="195" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C189" s="2">
         <v>3</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="E189" s="2" t="s">
         <v>11</v>
@@ -12672,50 +12658,50 @@
         <v>12</v>
       </c>
       <c r="G189" s="3" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="H189" s="4" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
     </row>
     <row r="190" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C190" s="2">
         <v>0</v>
       </c>
       <c r="D190" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="E190" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F190" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G190" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="H190" s="4" t="s">
         <v>468</v>
-      </c>
-      <c r="E190" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F190" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G190" s="3" t="s">
-        <v>469</v>
-      </c>
-      <c r="H190" s="4" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A191" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C191" s="2">
         <v>1</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E191" s="2" t="s">
         <v>11</v>
@@ -12724,50 +12710,50 @@
         <v>12</v>
       </c>
       <c r="G191" s="3" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="H191" s="4" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A192" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C192" s="2">
         <v>2</v>
       </c>
       <c r="D192" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="E192" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F192" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G192" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="H192" s="4" t="s">
         <v>473</v>
-      </c>
-      <c r="E192" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F192" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G192" s="3" t="s">
-        <v>474</v>
-      </c>
-      <c r="H192" s="4" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="193" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A193" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C193" s="2">
         <v>3</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E193" s="2" t="s">
         <v>11</v>
@@ -12776,180 +12762,180 @@
         <v>12</v>
       </c>
       <c r="G193" s="3" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="H193" s="4" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A194" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C194" s="2">
         <v>4</v>
       </c>
       <c r="D194" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="E194" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F194" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G194" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="H194" s="4" t="s">
         <v>478</v>
-      </c>
-      <c r="E194" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F194" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G194" s="3" t="s">
-        <v>479</v>
-      </c>
-      <c r="H194" s="4" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A195" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C195" s="2">
         <v>5</v>
       </c>
       <c r="D195" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="E195" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F195" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G195" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="H195" s="4" t="s">
         <v>481</v>
-      </c>
-      <c r="E195" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F195" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G195" s="3" t="s">
-        <v>482</v>
-      </c>
-      <c r="H195" s="4" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A196" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C196" s="2">
         <v>6</v>
       </c>
       <c r="D196" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="E196" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F196" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G196" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="H196" s="4" t="s">
         <v>484</v>
-      </c>
-      <c r="E196" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F196" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G196" s="3" t="s">
-        <v>485</v>
-      </c>
-      <c r="H196" s="4" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A197" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C197" s="2">
         <v>7</v>
       </c>
       <c r="D197" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="E197" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F197" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G197" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="H197" s="4" t="s">
         <v>487</v>
-      </c>
-      <c r="E197" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F197" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G197" s="3" t="s">
-        <v>488</v>
-      </c>
-      <c r="H197" s="4" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="198" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C198" s="2">
         <v>8</v>
       </c>
       <c r="D198" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="E198" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F198" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G198" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="H198" s="4" t="s">
         <v>490</v>
-      </c>
-      <c r="E198" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F198" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G198" s="3" t="s">
-        <v>491</v>
-      </c>
-      <c r="H198" s="4" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="199" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A199" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C199" s="2">
         <v>9</v>
       </c>
       <c r="D199" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="E199" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F199" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G199" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="H199" s="4" t="s">
         <v>493</v>
-      </c>
-      <c r="E199" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F199" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G199" s="3" t="s">
-        <v>494</v>
-      </c>
-      <c r="H199" s="4" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="200" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A200" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C200" s="2">
         <v>0</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="E200" s="2" t="s">
         <v>11</v>
@@ -12958,24 +12944,24 @@
         <v>12</v>
       </c>
       <c r="G200" s="3" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="H200" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="201" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A201" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C201" s="2">
         <v>1</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E201" s="2" t="s">
         <v>11</v>
@@ -12984,24 +12970,24 @@
         <v>12</v>
       </c>
       <c r="G201" s="3" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H201" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
     </row>
     <row r="202" spans="1:8" ht="135" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A202" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C202" s="2">
         <v>2</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E202" s="2" t="s">
         <v>11</v>
@@ -13010,102 +12996,102 @@
         <v>12</v>
       </c>
       <c r="G202" s="3" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="H202" s="7" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
     </row>
     <row r="203" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A203" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C203" s="2">
         <v>3</v>
       </c>
       <c r="D203" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="E203" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F203" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G203" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="H203" s="4" t="s">
         <v>503</v>
-      </c>
-      <c r="E203" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F203" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G203" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="H203" s="4" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A204" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C204" s="2">
         <v>4</v>
       </c>
       <c r="D204" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="E204" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F204" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G204" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="H204" s="4" t="s">
         <v>506</v>
-      </c>
-      <c r="E204" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F204" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G204" s="3" t="s">
-        <v>507</v>
-      </c>
-      <c r="H204" s="4" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="205" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A205" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C205" s="2">
         <v>0</v>
       </c>
       <c r="D205" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="E205" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F205" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G205" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="H205" s="4" t="s">
         <v>510</v>
-      </c>
-      <c r="E205" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F205" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G205" s="3" t="s">
-        <v>511</v>
-      </c>
-      <c r="H205" s="4" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="206" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A206" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C206" s="2">
         <v>1</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E206" s="2" t="s">
         <v>11</v>
@@ -13114,284 +13100,284 @@
         <v>12</v>
       </c>
       <c r="G206" s="3" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="H206" s="4" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A207" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C207" s="2">
         <v>2</v>
       </c>
       <c r="D207" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E207" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F207" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G207" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="H207" s="4" t="s">
         <v>515</v>
-      </c>
-      <c r="E207" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F207" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G207" s="3" t="s">
-        <v>516</v>
-      </c>
-      <c r="H207" s="4" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A208" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C208" s="2">
         <v>3</v>
       </c>
       <c r="D208" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="E208" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F208" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G208" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="H208" s="4" t="s">
         <v>518</v>
-      </c>
-      <c r="E208" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F208" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G208" s="3" t="s">
-        <v>519</v>
-      </c>
-      <c r="H208" s="4" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A209" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C209" s="2">
         <v>4</v>
       </c>
       <c r="D209" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="E209" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F209" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G209" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="H209" s="4" t="s">
         <v>521</v>
-      </c>
-      <c r="E209" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F209" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G209" s="3" t="s">
-        <v>522</v>
-      </c>
-      <c r="H209" s="4" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="210" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A210" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C210" s="2">
         <v>5</v>
       </c>
       <c r="D210" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="E210" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F210" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G210" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="H210" s="4" t="s">
         <v>524</v>
-      </c>
-      <c r="E210" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F210" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G210" s="3" t="s">
-        <v>525</v>
-      </c>
-      <c r="H210" s="4" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A211" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C211" s="2">
         <v>6</v>
       </c>
       <c r="D211" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="E211" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F211" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G211" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="H211" s="4" t="s">
         <v>527</v>
-      </c>
-      <c r="E211" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F211" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G211" s="3" t="s">
-        <v>528</v>
-      </c>
-      <c r="H211" s="4" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="212" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A212" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C212" s="2">
         <v>7</v>
       </c>
       <c r="D212" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="E212" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F212" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G212" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="H212" s="4" t="s">
         <v>530</v>
-      </c>
-      <c r="E212" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F212" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G212" s="3" t="s">
-        <v>531</v>
-      </c>
-      <c r="H212" s="4" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A213" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C213" s="2">
         <v>8</v>
       </c>
       <c r="D213" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="E213" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F213" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G213" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="H213" s="4" t="s">
         <v>533</v>
-      </c>
-      <c r="E213" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F213" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G213" s="3" t="s">
-        <v>534</v>
-      </c>
-      <c r="H213" s="4" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A214" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C214" s="2">
         <v>9</v>
       </c>
       <c r="D214" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="E214" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F214" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G214" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="H214" s="4" t="s">
         <v>536</v>
-      </c>
-      <c r="E214" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F214" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G214" s="3" t="s">
-        <v>537</v>
-      </c>
-      <c r="H214" s="4" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A215" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C215" s="2">
         <v>0</v>
       </c>
       <c r="D215" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="E215" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F215" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G215" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="H215" s="4" t="s">
         <v>540</v>
-      </c>
-      <c r="E215" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F215" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G215" s="3" t="s">
-        <v>541</v>
-      </c>
-      <c r="H215" s="4" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="216" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A216" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C216" s="2">
         <v>1</v>
       </c>
       <c r="D216" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="E216" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F216" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G216" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="H216" s="4" t="s">
         <v>543</v>
-      </c>
-      <c r="E216" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F216" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G216" s="3" t="s">
-        <v>544</v>
-      </c>
-      <c r="H216" s="4" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="217" spans="1:8" ht="165" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A217" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C217" s="2">
         <v>2</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="E217" s="2" t="s">
         <v>11</v>
@@ -13400,15 +13386,15 @@
         <v>12</v>
       </c>
       <c r="G217" s="3" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="H217" s="4" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="218" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A218" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B218" s="2" t="s">
         <v>258</v>
@@ -13417,24 +13403,24 @@
         <v>0</v>
       </c>
       <c r="D218" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="E218" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F218" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G218" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="H218" s="4" t="s">
         <v>548</v>
-      </c>
-      <c r="E218" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F218" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G218" s="3" t="s">
-        <v>549</v>
-      </c>
-      <c r="H218" s="4" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="219" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A219" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B219" s="2" t="s">
         <v>258</v>
@@ -13443,76 +13429,76 @@
         <v>1</v>
       </c>
       <c r="D219" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="E219" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F219" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G219" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="H219" s="4" t="s">
         <v>551</v>
-      </c>
-      <c r="E219" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F219" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G219" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="H219" s="4" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="220" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A220" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C220" s="2">
         <v>0</v>
       </c>
       <c r="D220" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="E220" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F220" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G220" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="H220" s="4" t="s">
         <v>555</v>
-      </c>
-      <c r="E220" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F220" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G220" s="3" t="s">
-        <v>556</v>
-      </c>
-      <c r="H220" s="4" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A221" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C221" s="2">
         <v>1</v>
       </c>
       <c r="D221" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="E221" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F221" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G221" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="H221" s="4" t="s">
         <v>558</v>
-      </c>
-      <c r="E221" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F221" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G221" s="3" t="s">
-        <v>559</v>
-      </c>
-      <c r="H221" s="4" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="222" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A222" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B222" s="2" t="s">
         <v>249</v>
@@ -13521,24 +13507,24 @@
         <v>0</v>
       </c>
       <c r="D222" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="E222" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F222" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G222" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="H222" s="4" t="s">
         <v>561</v>
-      </c>
-      <c r="E222" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F222" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G222" s="3" t="s">
-        <v>562</v>
-      </c>
-      <c r="H222" s="4" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="223" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A223" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B223" s="2" t="s">
         <v>249</v>
@@ -13547,24 +13533,24 @@
         <v>1</v>
       </c>
       <c r="D223" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="E223" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F223" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G223" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="H223" s="4" t="s">
         <v>564</v>
-      </c>
-      <c r="E223" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F223" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G223" s="3" t="s">
-        <v>565</v>
-      </c>
-      <c r="H223" s="4" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A224" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B224" s="2" t="s">
         <v>249</v>
@@ -13573,7 +13559,7 @@
         <v>2</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="E224" s="2" t="s">
         <v>11</v>
@@ -13582,7 +13568,7 @@
         <v>12</v>
       </c>
       <c r="G224" s="3" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="H224" s="4" t="s">
         <v>14</v>
@@ -13590,7 +13576,7 @@
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A225" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B225" s="2" t="s">
         <v>249</v>
@@ -13599,7 +13585,7 @@
         <v>3</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="E225" s="2" t="s">
         <v>11</v>
@@ -13608,7 +13594,7 @@
         <v>12</v>
       </c>
       <c r="G225" s="3" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="H225" s="4" t="s">
         <v>14</v>
@@ -13616,42 +13602,42 @@
     </row>
     <row r="226" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A226" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C226" s="2">
         <v>0</v>
       </c>
       <c r="D226" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="E226" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F226" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G226" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="H226" s="4" t="s">
         <v>572</v>
-      </c>
-      <c r="E226" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F226" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G226" s="3" t="s">
-        <v>573</v>
-      </c>
-      <c r="H226" s="4" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="227" spans="1:8" ht="165" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A227" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C227" s="2">
         <v>1</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="E227" s="2" t="s">
         <v>11</v>
@@ -13660,50 +13646,50 @@
         <v>12</v>
       </c>
       <c r="G227" s="3" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="H227" s="4" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="228" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A228" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C228" s="2">
         <v>0</v>
       </c>
       <c r="D228" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="E228" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F228" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G228" s="3" t="s">
+        <v>576</v>
+      </c>
+      <c r="H228" s="4" t="s">
         <v>577</v>
-      </c>
-      <c r="E228" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F228" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G228" s="3" t="s">
-        <v>578</v>
-      </c>
-      <c r="H228" s="4" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="229" spans="1:8" ht="180" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A229" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C229" s="2">
         <v>1</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E229" s="2" t="s">
         <v>11</v>
@@ -13712,24 +13698,24 @@
         <v>12</v>
       </c>
       <c r="G229" s="3" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="H229" s="4" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A230" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C230" s="2">
         <v>2</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E230" s="2" t="s">
         <v>11</v>
@@ -13738,24 +13724,24 @@
         <v>12</v>
       </c>
       <c r="G230" s="3" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="H230" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A231" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C231" s="2">
         <v>3</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E231" s="2" t="s">
         <v>11</v>
@@ -13764,24 +13750,24 @@
         <v>12</v>
       </c>
       <c r="G231" s="3" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="H231" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A232" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C232" s="2">
         <v>0</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="E232" s="2" t="s">
         <v>11</v>
@@ -13790,24 +13776,24 @@
         <v>12</v>
       </c>
       <c r="G232" s="3" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="H232" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A233" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C233" s="2">
         <v>1</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="E233" s="2" t="s">
         <v>11</v>
@@ -13816,7 +13802,7 @@
         <v>12</v>
       </c>
       <c r="G233" s="3" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="H233" s="4" t="s">
         <v>14</v>
@@ -13824,16 +13810,16 @@
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A234" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C234" s="2">
         <v>0</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E234" s="2" t="s">
         <v>11</v>
@@ -13842,7 +13828,7 @@
         <v>12</v>
       </c>
       <c r="G234" s="5" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="H234" s="4" t="s">
         <v>14</v>
@@ -13850,16 +13836,16 @@
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A235" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C235" s="2">
         <v>1</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="E235" s="2" t="s">
         <v>11</v>
@@ -13868,7 +13854,7 @@
         <v>12</v>
       </c>
       <c r="G235" s="5" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="H235" s="4" t="s">
         <v>14</v>
@@ -13876,16 +13862,16 @@
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A236" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C236" s="2">
         <v>2</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E236" s="2" t="s">
         <v>11</v>
@@ -13894,7 +13880,7 @@
         <v>12</v>
       </c>
       <c r="G236" s="3" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="H236" s="4" t="s">
         <v>14</v>
@@ -13902,16 +13888,16 @@
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A237" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C237" s="2">
         <v>3</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="E237" s="2" t="s">
         <v>11</v>
@@ -13920,7 +13906,7 @@
         <v>12</v>
       </c>
       <c r="G237" s="3" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="H237" s="4" t="s">
         <v>14</v>
@@ -13946,301 +13932,301 @@
         <v>12</v>
       </c>
       <c r="G238" s="3" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="H238" s="4" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="239" spans="1:8" ht="360" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A239" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C239" s="2">
         <v>1001</v>
       </c>
       <c r="D239" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="E239" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F239" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G239" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H239" s="4" t="s">
         <v>601</v>
-      </c>
-      <c r="E239" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F239" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G239" s="3" t="s">
-        <v>602</v>
-      </c>
-      <c r="H239" s="4" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="240" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A240" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C240" s="2">
         <v>1001</v>
       </c>
       <c r="D240" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="E240" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F240" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G240" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="H240" s="4" t="s">
         <v>604</v>
-      </c>
-      <c r="E240" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F240" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G240" s="3" t="s">
-        <v>605</v>
-      </c>
-      <c r="H240" s="4" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="241" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A241" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C241" s="2">
         <v>1001</v>
       </c>
       <c r="D241" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="E241" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F241" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G241" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="H241" s="4" t="s">
         <v>607</v>
-      </c>
-      <c r="E241" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F241" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G241" s="3" t="s">
-        <v>608</v>
-      </c>
-      <c r="H241" s="4" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A242" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C242" s="2">
         <v>1002</v>
       </c>
       <c r="D242" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="E242" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F242" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G242" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="H242" s="4" t="s">
         <v>610</v>
-      </c>
-      <c r="E242" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F242" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G242" s="3" t="s">
-        <v>611</v>
-      </c>
-      <c r="H242" s="4" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="243" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A243" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="C243" s="2">
         <v>1000</v>
       </c>
       <c r="D243" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="E243" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F243" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G243" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="H243" s="4" t="s">
         <v>614</v>
-      </c>
-      <c r="E243" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F243" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G243" s="3" t="s">
-        <v>615</v>
-      </c>
-      <c r="H243" s="4" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="244" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A244" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="C244" s="2">
         <v>1001</v>
       </c>
       <c r="D244" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="E244" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F244" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G244" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="H244" s="4" t="s">
         <v>617</v>
-      </c>
-      <c r="E244" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F244" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G244" s="3" t="s">
-        <v>618</v>
-      </c>
-      <c r="H244" s="4" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="245" spans="1:8" ht="150" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A245" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C245" s="2">
         <v>1003</v>
       </c>
       <c r="D245" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="E245" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F245" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G245" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="H245" s="4" t="s">
         <v>620</v>
-      </c>
-      <c r="E245" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F245" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G245" s="3" t="s">
-        <v>621</v>
-      </c>
-      <c r="H245" s="4" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="246" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A246" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C246" s="2">
         <v>1003</v>
       </c>
       <c r="D246" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="E246" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F246" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G246" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="H246" s="4" t="s">
         <v>623</v>
-      </c>
-      <c r="E246" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F246" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G246" s="3" t="s">
-        <v>624</v>
-      </c>
-      <c r="H246" s="4" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A247" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C247" s="2">
         <v>1000</v>
       </c>
       <c r="D247" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="E247" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F247" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G247" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="H247" s="4" t="s">
         <v>626</v>
-      </c>
-      <c r="E247" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F247" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G247" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="H247" s="4" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A248" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C248" s="2">
         <v>1001</v>
       </c>
       <c r="D248" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="E248" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F248" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G248" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="H248" s="4" t="s">
         <v>629</v>
-      </c>
-      <c r="E248" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F248" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G248" s="3" t="s">
-        <v>630</v>
-      </c>
-      <c r="H248" s="4" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="249" spans="1:8" ht="165" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A249" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C249" s="2">
         <v>1002</v>
       </c>
       <c r="D249" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="E249" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F249" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G249" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="H249" s="4" t="s">
         <v>632</v>
-      </c>
-      <c r="E249" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F249" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G249" s="3" t="s">
-        <v>633</v>
-      </c>
-      <c r="H249" s="4" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A250" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B250" s="2" t="s">
         <v>249</v>
@@ -14249,7 +14235,7 @@
         <v>1002</v>
       </c>
       <c r="D250" s="2" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="E250" s="2" t="s">
         <v>11</v>
@@ -14258,15 +14244,15 @@
         <v>12</v>
       </c>
       <c r="G250" s="3" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="H250" s="4" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A251" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B251" s="2" t="s">
         <v>249</v>
@@ -14275,7 +14261,7 @@
         <v>1003</v>
       </c>
       <c r="D251" s="2" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="E251" s="2" t="s">
         <v>11</v>
@@ -14284,102 +14270,102 @@
         <v>12</v>
       </c>
       <c r="G251" s="3" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H251" s="4" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="252" spans="1:8" ht="135" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A252" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C252" s="2">
         <v>1001</v>
       </c>
       <c r="D252" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="E252" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F252" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G252" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="H252" s="4" t="s">
         <v>637</v>
-      </c>
-      <c r="E252" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F252" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G252" s="3" t="s">
-        <v>638</v>
-      </c>
-      <c r="H252" s="4" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="253" spans="1:8" ht="180" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A253" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C253" s="2">
         <v>1001</v>
       </c>
       <c r="D253" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="E253" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F253" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G253" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="H253" s="4" t="s">
         <v>640</v>
-      </c>
-      <c r="E253" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F253" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G253" s="3" t="s">
-        <v>641</v>
-      </c>
-      <c r="H253" s="4" t="s">
-        <v>642</v>
       </c>
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A254" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C254" s="2">
         <v>1000</v>
       </c>
       <c r="D254" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="E254" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F254" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G254" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="H254" s="4" t="s">
         <v>644</v>
-      </c>
-      <c r="E254" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F254" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G254" s="3" t="s">
-        <v>645</v>
-      </c>
-      <c r="H254" s="4" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A255" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C255" s="2">
         <v>1001</v>
       </c>
       <c r="D255" s="2" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="E255" s="2" t="s">
         <v>11</v>
@@ -14388,10 +14374,10 @@
         <v>12</v>
       </c>
       <c r="G255" s="3" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="H255" s="4" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>